<commit_message>
Completed the analysis on interpolation implemented.
</commit_message>
<xml_diff>
--- a/Regression_mterics_with_radius_0.0015.xlsx
+++ b/Regression_mterics_with_radius_0.0015.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9990995917218514</v>
+        <v>0.9039155943081556</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9968355367942606</v>
+        <v>0.9987679826329908</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9967834030700745</v>
+        <v>0.9988129942789321</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9997935382103196</v>
+        <v>0.9917829357034532</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9978041593610564</v>
+        <v>0.9964546376082618</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9733558092359214</v>
+        <v>0.9935453628626348</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9943915684091371</v>
+        <v>0.9929116505919509</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9970397268474199</v>
+        <v>0.8785558378176582</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.61059602862224e-05</v>
+        <v>0.007054299581795931</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0001983250258490443</v>
+        <v>7.72136845625937e-05</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002053879579761997</v>
+        <v>7.579336670460179e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>1.212119286719826e-06</v>
+        <v>4.824167990591377e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001349583471892402</v>
+        <v>6.705630948999897e-05</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003999836917500943</v>
+        <v>9.689725993666798e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>6.919930228832527e-07</v>
+        <v>8.745918762542715e-07</v>
       </c>
       <c r="I3" t="n">
-        <v>3.279455661773682</v>
+        <v>134.5385284423828</v>
       </c>
     </row>
     <row r="4">
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.008130556903779507</v>
+        <v>0.08398988097906113</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01408279221504927</v>
+        <v>0.008787131868302822</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01433136314153671</v>
+        <v>0.00870593823492527</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001100962865166366</v>
+        <v>0.006945623084902763</v>
       </c>
       <c r="F4" t="n">
-        <v>0.009837827645242214</v>
+        <v>0.008144588209688663</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01999959163367748</v>
+        <v>0.009843640960752964</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0008318611653521657</v>
+        <v>0.0009351961780339479</v>
       </c>
       <c r="I4" t="n">
-        <v>1.810926795005798</v>
+        <v>11.5990743637085</v>
       </c>
     </row>
     <row r="5">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001059245085343719</v>
+        <v>0.01926547475159168</v>
       </c>
       <c r="C5" t="n">
-        <v>0.002013444434851408</v>
+        <v>0.002964772982522845</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002079891972243786</v>
+        <v>0.003025685669854283</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0001713910169200972</v>
+        <v>0.002364977030083537</v>
       </c>
       <c r="F5" t="n">
-        <v>0.001422049128450453</v>
+        <v>0.002785254968330264</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003019498195499182</v>
+        <v>0.003383800620213151</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001340980379609391</v>
+        <v>0.0003872609813697636</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2143738269805908</v>
+        <v>2.974501132965088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>